<commit_message>
change S+LFM to S/LFM in taxonomy
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Italy_COM.xlsx
+++ b/com_mapping_schemes/mapping_Italy_COM.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C35F19-DBB3-2C4C-8DF9-C8E5C6B7BE14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="18380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -41,7 +47,7 @@
 1.6% MUR+STRUB/LWAL+CDN/H:1/Offices
 3.8% MUR+STRUB/LWAL+CDN/H:2/Offices
 2.4% MUR+STRUB/LWAL+CDN/HBET:3-5/Offices
-0.6% S+LFM/CDL/HBET:3-5/Offices
+0.6% S/LFM/CDL/HBET:3-5/Offices
 0.0% MUR+CL/LWAL+CDN/H:1/Offices
 0.0% MUR+CL/LWAL+CDN/H:2/Offices
 0.0% MUR+CL/LWAL+CDN/HBET:6-/Offices
@@ -66,7 +72,7 @@
 39.9% MUR+STRUB/LWAL+CDN/H:1/Trade
 12.7% MUR+STRUB/LWAL+CDN/H:2/Trade
 0.0% MUR+STRUB/LWAL+CDN/HBET:3-5/Trade
-0.0% S+LFM/CDL/HBET:3-5/Trade
+0.0% S/LFM/CDL/HBET:3-5/Trade
 3.5% MUR+CL/LWAL+CDN/H:1/Trade
 0.5% MUR+CL/LWAL+CDN/H:2/Trade
 0.0% MUR+CL/LWAL+CDN/HBET:6-/Trade
@@ -91,7 +97,7 @@
  32.2% MUR+STRUB/LWAL+CDN/H:1/Hotels
  10.2% MUR+STRUB/LWAL+CDN/H:2/Hotels
  19.6% MUR+STRUB/LWAL+CDN/HBET:3-5/Hotels
- 0.0% S+LFM/CDL/HBET:3-5/Hotels
+ 0.0% S/LFM/CDL/HBET:3-5/Hotels
  0.0% MUR+CL/LWAL+CDN/H:1/Hotels
  0.0% MUR+CL/LWAL+CDN/H:2/Hotels
  0.4% MUR+CL/LWAL+CDN/HBET:6-/Hotels
@@ -103,8 +109,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,10 +162,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -167,6 +176,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -213,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +262,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +314,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,14 +507,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,14 +532,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="365" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update Italy commercial model with LFM+CDL correction
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Italy_COM.xlsx
+++ b/com_mapping_schemes/mapping_Italy_COM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C35F19-DBB3-2C4C-8DF9-C8E5C6B7BE14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715481E6-B4A5-6940-8DE2-8F3180420248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="18380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 1.6% MUR+STRUB/LWAL+CDN/H:1/Offices
 3.8% MUR+STRUB/LWAL+CDN/H:2/Offices
 2.4% MUR+STRUB/LWAL+CDN/HBET:3-5/Offices
-0.6% S/LFM/CDL/HBET:3-5/Offices
+0.6% S/LFM+CDL/HBET:3-5/Offices
 0.0% MUR+CL/LWAL+CDN/H:1/Offices
 0.0% MUR+CL/LWAL+CDN/H:2/Offices
 0.0% MUR+CL/LWAL+CDN/HBET:6-/Offices
@@ -72,7 +72,7 @@
 39.9% MUR+STRUB/LWAL+CDN/H:1/Trade
 12.7% MUR+STRUB/LWAL+CDN/H:2/Trade
 0.0% MUR+STRUB/LWAL+CDN/HBET:3-5/Trade
-0.0% S/LFM/CDL/HBET:3-5/Trade
+0.0% S/LFM+CDL/HBET:3-5/Trade
 3.5% MUR+CL/LWAL+CDN/H:1/Trade
 0.5% MUR+CL/LWAL+CDN/H:2/Trade
 0.0% MUR+CL/LWAL+CDN/HBET:6-/Trade
@@ -97,7 +97,7 @@
  32.2% MUR+STRUB/LWAL+CDN/H:1/Hotels
  10.2% MUR+STRUB/LWAL+CDN/H:2/Hotels
  19.6% MUR+STRUB/LWAL+CDN/HBET:3-5/Hotels
- 0.0% S/LFM/CDL/HBET:3-5/Hotels
+ 0.0% S/LFM+CDL/HBET:3-5/Hotels
  0.0% MUR+CL/LWAL+CDN/H:1/Hotels
  0.0% MUR+CL/LWAL+CDN/H:2/Hotels
  0.4% MUR+CL/LWAL+CDN/HBET:6-/Hotels
@@ -511,7 +511,7 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
correction S/LFM mapping Italy commercial
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Italy_COM.xlsx
+++ b/com_mapping_schemes/mapping_Italy_COM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715481E6-B4A5-6940-8DE2-8F3180420248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F2D579-4CAA-1A48-9A73-DC7CF07A42B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="20280" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_com" sheetId="1" r:id="rId1"/>
@@ -47,13 +47,12 @@
 1.6% MUR+STRUB/LWAL+CDN/H:1/Offices
 3.8% MUR+STRUB/LWAL+CDN/H:2/Offices
 2.4% MUR+STRUB/LWAL+CDN/HBET:3-5/Offices
-0.6% S/LFM+CDL/HBET:3-5/Offices
 0.0% MUR+CL/LWAL+CDN/H:1/Offices
 0.0% MUR+CL/LWAL+CDN/H:2/Offices
 0.0% MUR+CL/LWAL+CDN/HBET:6-/Offices
 0.0% MUR+STDRE/LWAL+CDN/HBET:3-5/Offices
 0.0% MUR+STDRE/LWAL+CDN/HBET:6-/Offices
-0.0% S/LFM+CDL/HBET:3-5/Offices</t>
+0.6% S/LFM+CDL/HBET:3-5/Offices</t>
   </si>
   <si>
     <t>2.4% CR/LFINF+CDL/H:1/Trade
@@ -72,7 +71,6 @@
 39.9% MUR+STRUB/LWAL+CDN/H:1/Trade
 12.7% MUR+STRUB/LWAL+CDN/H:2/Trade
 0.0% MUR+STRUB/LWAL+CDN/HBET:3-5/Trade
-0.0% S/LFM+CDL/HBET:3-5/Trade
 3.5% MUR+CL/LWAL+CDN/H:1/Trade
 0.5% MUR+CL/LWAL+CDN/H:2/Trade
 0.0% MUR+CL/LWAL+CDN/HBET:6-/Trade
@@ -97,7 +95,6 @@
  32.2% MUR+STRUB/LWAL+CDN/H:1/Hotels
  10.2% MUR+STRUB/LWAL+CDN/H:2/Hotels
  19.6% MUR+STRUB/LWAL+CDN/HBET:3-5/Hotels
- 0.0% S/LFM+CDL/HBET:3-5/Hotels
  0.0% MUR+CL/LWAL+CDN/H:1/Hotels
  0.0% MUR+CL/LWAL+CDN/H:2/Hotels
  0.4% MUR+CL/LWAL+CDN/HBET:6-/Hotels
@@ -511,7 +508,7 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -532,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="365" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" ht="350" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Update Italy commercial mapping and area to match CR typologies in 2011 census
</commit_message>
<xml_diff>
--- a/com_mapping_schemes/mapping_Italy_COM.xlsx
+++ b/com_mapping_schemes/mapping_Italy_COM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/com_mapping_schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F2D579-4CAA-1A48-9A73-DC7CF07A42B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F611590D-05CE-7649-8131-81F7B490709E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="20280" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,38 +31,38 @@
     <t>Hotels</t>
   </si>
   <si>
-    <t>2.9% CR/LFINF+CDL/H:1/Offices
-10.0% CR/LFINF+CDL/H:2/Offices
-7.0% CR/LFINF+CDL/HBET:3-5/Offices
-3.0% CR/LFINF+CDL/HBET:6-/Offices
-17.5% CR/LFINF+CDN/H:1/Offices
-10.2% CR/LFINF+CDN/H:2/Offices
-27.9% CR/LFINF+CDN/HBET:3-5/Offices
-8.2% CR/LFINF+CDN/HBET:6-/Offices
-0.6% MCF/LWAL+CDL/H:1/Offices
-1.1% MCF/LWAL+CDL/H:2/Offices
-0.5% MCF/LWAL+CDL/HBET:3-5/Offices
-0.0% MCF/LWAL+CDL/HBET:6-/Offices
-2.7% MUR+CL/LWAL+CDN/HBET:3-5/Offices
-1.6% MUR+STRUB/LWAL+CDN/H:1/Offices
-3.8% MUR+STRUB/LWAL+CDN/H:2/Offices
-2.4% MUR+STRUB/LWAL+CDN/HBET:3-5/Offices
-0.0% MUR+CL/LWAL+CDN/H:1/Offices
-0.0% MUR+CL/LWAL+CDN/H:2/Offices
-0.0% MUR+CL/LWAL+CDN/HBET:6-/Offices
-0.0% MUR+STDRE/LWAL+CDN/HBET:3-5/Offices
-0.0% MUR+STDRE/LWAL+CDN/HBET:6-/Offices
-0.6% S/LFM+CDL/HBET:3-5/Offices</t>
+    <t>3.2% CR/LFINF+CDL3/H:1/Hotels
+ 2.1% CR/LFINF+CDL3/H:2/Hotels
+ 2.3% CR/LFINF+CDL3/HBET:3-5/Hotels
+ 0.2% CR/LFINF+CDL3/HBET:6-/Hotels
+ 8.0% CR/LFINF+CDL2/H:1/Hotels
+ 2.9% CR/LFINF+CDL2/H:2/Hotels
+ 9.0% CR/LFINF+CDL2/HBET:3-5/Hotels
+ 3.0% CR/LFINF+CDL2/HBET:6-/Hotels
+ 1.1% MCF/LWAL+CDL/H:1/Hotels
+ 0.6% MCF/LWAL+CDL/H:2/Hotels
+ 0.4% MCF/LWAL+CDL/HBET:3-5/Hotels
+ 0.0% MCF/LWAL+CDL/HBET:6-/Hotels
+ 2.7% MUR+CL/LWAL+CDN/HBET:3-5/Hotels
+ 32.2% MUR+STRUB/LWAL+CDN/H:1/Hotels
+ 10.2% MUR+STRUB/LWAL+CDN/H:2/Hotels
+ 19.6% MUR+STRUB/LWAL+CDN/HBET:3-5/Hotels
+ 0.0% MUR+CL/LWAL+CDN/H:1/Hotels
+ 0.0% MUR+CL/LWAL+CDN/H:2/Hotels
+ 0.4% MUR+CL/LWAL+CDN/HBET:6-/Hotels
+ 0.1% MUR+STDRE/LWAL+CDN/HBET:3-5/Hotels
+ 0.0% MUR+STDRE/LWAL+CDN/HBET:6-/Hotels
+ 2.0% S/LFM+CDL/HBET:3-5/Hotels</t>
   </si>
   <si>
-    <t>2.4% CR/LFINF+CDL/H:1/Trade
-7.3% CR/LFINF+CDL/H:2/Trade
-0.0% CR/LFINF+CDL/HBET:3-5/Trade
-0.0% CR/LFINF+CDL/HBET:6-/Trade
-16.1% CR/LFINF+CDN/H:1/Trade
-14.9% CR/LFINF+CDN/H:2/Trade
-0.0% CR/LFINF+CDN/HBET:3-5/Trade
-0.0% CR/LFINF+CDN/HBET:6-/Trade
+    <t>2.4% CR/LFINF+CDL3/H:1/Trade
+7.3% CR/LFINF+CDL3/H:2/Trade
+0.0% CR/LFINF+CDL3/HBET:3-5/Trade
+0.0% CR/LFINF+CDL3/HBET:6-/Trade
+16.1% CR/LFINF+CDL2/H:1/Trade
+14.9% CR/LFINF+CDL2/H:2/Trade
+0.0% CR/LFINF+CDL2/HBET:3-5/Trade
+0.0% CR/LFINF+CDL2/HBET:6-/Trade
 1.4% MCF/LWAL+CDL/H:1/Trade
 1.3% MCF/LWAL+CDL/H:2/Trade
 0.0% MCF/LWAL+CDL/HBET:3-5/Trade
@@ -79,28 +79,28 @@
 0.0% S/LFM+CDL/HBET:3-5/Trade</t>
   </si>
   <si>
-    <t>3.2% CR/LFINF+CDL/H:1/Hotels
- 2.1% CR/LFINF+CDL/H:2/Hotels
- 2.3% CR/LFINF+CDL/HBET:3-5/Hotels
- 0.2% CR/LFINF+CDL/HBET:6-/Hotels
- 8.0% CR/LFINF+CDN/H:1/Hotels
- 2.9% CR/LFINF+CDN/H:2/Hotels
- 9.0% CR/LFINF+CDN/HBET:3-5/Hotels
- 3.0% CR/LFINF+CDN/HBET:6-/Hotels
- 1.1% MCF/LWAL+CDL/H:1/Hotels
- 0.6% MCF/LWAL+CDL/H:2/Hotels
- 0.4% MCF/LWAL+CDL/HBET:3-5/Hotels
- 0.0% MCF/LWAL+CDL/HBET:6-/Hotels
- 2.7% MUR+CL/LWAL+CDN/HBET:3-5/Hotels
- 32.2% MUR+STRUB/LWAL+CDN/H:1/Hotels
- 10.2% MUR+STRUB/LWAL+CDN/H:2/Hotels
- 19.6% MUR+STRUB/LWAL+CDN/HBET:3-5/Hotels
- 0.0% MUR+CL/LWAL+CDN/H:1/Hotels
- 0.0% MUR+CL/LWAL+CDN/H:2/Hotels
- 0.4% MUR+CL/LWAL+CDN/HBET:6-/Hotels
- 0.1% MUR+STDRE/LWAL+CDN/HBET:3-5/Hotels
- 0.0% MUR+STDRE/LWAL+CDN/HBET:6-/Hotels
- 2.0% S/LFM+CDL/HBET:3-5/Hotels</t>
+    <t>2.9% CR/LFINF+CDL3/H:1/Offices
+10.0% CR/LFINF+CDL3/H:2/Offices
+7.0% CR/LFINF+CDL3/HBET:3-5/Offices
+3.0% CR/LFINF+CDL3/HBET:6-/Offices
+17.5% CR/LFINF+CDL2/H:1/Offices
+10.2% CR/LFINF+CDL2/H:2/Offices
+27.9% CR/LFINF+CDL2/HBET:3-5/Offices
+8.2% CR/LFINF+CDL2/HBET:6-/Offices
+0.6% MCF/LWAL+CDL/H:1/Offices
+1.1% MCF/LWAL+CDL/H:2/Offices
+0.5% MCF/LWAL+CDL/HBET:3-5/Offices
+0.0% MCF/LWAL+CDL/HBET:6-/Offices
+2.7% MUR+CL/LWAL+CDN/HBET:3-5/Offices
+1.6% MUR+STRUB/LWAL+CDN/H:1/Offices
+3.8% MUR+STRUB/LWAL+CDN/H:2/Offices
+2.4% MUR+STRUB/LWAL+CDN/HBET:3-5/Offices
+0.0% MUR+CL/LWAL+CDN/H:1/Offices
+0.0% MUR+CL/LWAL+CDN/H:2/Offices
+0.0% MUR+CL/LWAL+CDN/HBET:6-/Offices
+0.0% MUR+STDRE/LWAL+CDN/HBET:3-5/Offices
+0.0% MUR+STDRE/LWAL+CDN/HBET:6-/Offices
+0.6% S/LFM+CDL/HBET:3-5/Offices</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -531,13 +531,13 @@
     </row>
     <row r="2" spans="2:4" ht="350" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>